<commit_message>
Fix 29: clean phone numbers
</commit_message>
<xml_diff>
--- a/29.climbodachi/extracted_data/29.Data.xlsx
+++ b/29.climbodachi/extracted_data/29.Data.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Upwork\Task01\Multiple_Directories_Web_scraping\29.climbodachi\extracted_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA991EF2-D1F7-4BB3-9DB5-FA63349BA43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -31,6 +26,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>openHours</t>
+  </si>
+  <si>
     <t>phone</t>
   </si>
   <si>
@@ -61,7 +59,10 @@
     <t>Opening Hours: Mon Closed; Tue-Fri 4pm-9pm; Sat-Sun 12pm-7pm</t>
   </si>
   <si>
-    <t> +60 8 966 5448</t>
+    <t> Mon Closed; Tue-Fri 4pm-9pm; Sat-Sun 12pm-7pm</t>
+  </si>
+  <si>
+    <t>+60 8 966 5448</t>
   </si>
   <si>
     <t>https://www.facebook.com/bananaclimbinggym/</t>
@@ -76,7 +77,10 @@
     <t>Opening Hours: Mon-Fri 2.30pm-10pm; Sat 10.30am-6pm; Sun Closed</t>
   </si>
   <si>
-    <t> +60 38 023 4948</t>
+    <t> Mon-Fri 2.30pm-10pm; Sat 10.30am-6pm; Sun Closed</t>
+  </si>
+  <si>
+    <t>+60 38 023 4948</t>
   </si>
   <si>
     <t>https://www.bolderventures.com.my/</t>
@@ -112,7 +116,10 @@
     <t>Opening Hours: Mon-Fri 12pm-11pm; Sat-Sun 10am-8pm</t>
   </si>
   <si>
-    <t> +60 37 726 0410</t>
+    <t> Mon-Fri 12pm-11pm; Sat-Sun 10am-8pm</t>
+  </si>
+  <si>
+    <t>+60 37 726 0410</t>
   </si>
   <si>
     <t>http://www.camp5.com/</t>
@@ -127,7 +134,10 @@
     <t>Opening Hours: Mon-Sun 10am-10pm</t>
   </si>
   <si>
-    <t> +60 32 201 4360</t>
+    <t> Mon-Sun 10am-10pm</t>
+  </si>
+  <si>
+    <t>+60 32 201 4360</t>
   </si>
   <si>
     <t>Camp5 Climbing Gym – Jumpa</t>
@@ -136,7 +146,7 @@
     <t>3rd Floor, Jumpa Sungai Wang Mall, Jalan Sultan Ismail, Bukit Bintang, 59200 Kuala Lumpur, Malaysia</t>
   </si>
   <si>
-    <t> +60 32 713 7128/29</t>
+    <t>+60 32 713 7128/29</t>
   </si>
   <si>
     <t>Camp5 Climbing Gym – Paradigm</t>
@@ -145,7 +155,7 @@
     <t>Paradigm Mall, 7F-08 Level 7, Skudai, Jalan Bertingkat Skudai, 81200 Johor Bahru, Johor, Malaysia</t>
   </si>
   <si>
-    <t> +60 72 32 7783</t>
+    <t>+60 72 32 7783</t>
   </si>
   <si>
     <t>Camp5 Climbing Gym – Utropolis</t>
@@ -154,7 +164,7 @@
     <t>Lot UG- D1a, Utropolis Marketplace, Jalan Kontraktor U1/14, Sek U1, 40150 Shah Alam, Selangor, Malaysia</t>
   </si>
   <si>
-    <t> +60 35 036 0160</t>
+    <t>+60 35 036 0160</t>
   </si>
   <si>
     <t>Camp5 KL East</t>
@@ -178,7 +188,10 @@
     <t>Opening Hours: Mon-Sun 10am-10pm</t>
   </si>
   <si>
-    <t xml:space="preserve"> +60 16 776 7733</t>
+    <t xml:space="preserve"> Mon-Sun 10am-10pm</t>
+  </si>
+  <si>
+    <t>+60 16 776 7733</t>
   </si>
   <si>
     <t>https://www.facebook.com/HangOutClimbingGym</t>
@@ -188,9 +201,6 @@
   </si>
   <si>
     <t>1-L5-28, Metro Avenue, Lintang Hajjah Rehmah, 11600 Jelutong, Pulau Pinang, Malaysia</t>
-  </si>
-  <si>
-    <t> +60 16 776 7733</t>
   </si>
   <si>
     <t>KilmbZone</t>
@@ -218,7 +228,10 @@
     <t>Opening Hours: Mon 6pm-11pm; Tue-Fri 2pm-11pm; Sat-Sun 10am-7pm</t>
   </si>
   <si>
-    <t> +60 34 142 0698</t>
+    <t> Mon 6pm-11pm; Tue-Fri 2pm-11pm; Sat-Sun 10am-7pm</t>
+  </si>
+  <si>
+    <t>+60 34 142 0698</t>
   </si>
   <si>
     <t>https://madmonkeyz.my/</t>
@@ -258,7 +271,10 @@
     <t>Opening Hours: Mon Closed; Tue-Thu 12pm-9pm; Sat-Sun 11am-9pm</t>
   </si>
   <si>
-    <t> +60 19 716 6222</t>
+    <t xml:space="preserve"> Mon Closed; Tue-Thu 12pm-9pm; Sat-Sun 11am-9pm</t>
+  </si>
+  <si>
+    <t>+60 19 716 6222</t>
   </si>
   <si>
     <t>http://www.petitoutdoor.com.my/</t>
@@ -270,7 +286,7 @@
     <t>170-07-12A, Plaza Gurney, Persiaran Gurney, 10250 George Town, Penang, Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve"> +60 4228 3300</t>
+    <t>+60 4228 3300</t>
   </si>
   <si>
     <t>https://www.projectrock.com.my/</t>
@@ -282,7 +298,7 @@
     <t>L1.10, IKEA Batu Kawan – Link Building, Aspen Vision City, Lebuhraya Bandar Cassia, 14110 Batu Kawan, Pulau Pinang, Malaysia</t>
   </si>
   <si>
-    <t> +60 10 948 3009</t>
+    <t>+60 10 948 3009</t>
   </si>
   <si>
     <t>Putrajaya Challenge Park</t>
@@ -294,7 +310,10 @@
     <t>Opening Hours: Mon-Tue 10am-8pm; Wed 10am-10pm; Thu 10am-8pm; Fri 10am-12.30pm, 3pm-10pm; Sat-Sun 10am-8pm</t>
   </si>
   <si>
-    <t> +60 38 887 7000</t>
+    <t> Mon-Tue 10am-8pm; Wed 10am-10pm; Thu 10am-8pm; Fri 10am-12.30pm, 3pm-10pm; Sat-Sun 10am-8pm</t>
+  </si>
+  <si>
+    <t>+60 38 887 7000</t>
   </si>
   <si>
     <t>https://www.facebook.com/Putrajaya.Challenge.Park/</t>
@@ -309,7 +328,10 @@
     <t>Opening Hours: Mon Closed; Tue-Fri 6pm-11.30pm; Sat-Sun 10am-10pm</t>
   </si>
   <si>
-    <t> +60 19 772 9338</t>
+    <t> Mon Closed; Tue-Fri 6pm-11.30pm; Sat-Sun 10am-10pm</t>
+  </si>
+  <si>
+    <t>+60 19 772 9338</t>
   </si>
   <si>
     <t>https://www.facebook.com/Rockworldjb/</t>
@@ -324,7 +346,10 @@
     <t>Opening Hours: Mon-Sun 11am-10pm</t>
   </si>
   <si>
-    <t> +60 35 524 1020</t>
+    <t> Mon-Sun 11am-10pm</t>
+  </si>
+  <si>
+    <t>+60 35 524 1020</t>
   </si>
   <si>
     <t>http://www.rockybasecamp.com/</t>
@@ -336,7 +361,7 @@
     <t>F102A, Level 1, Lot, Taman Desa Tebrau, 81100 Johor Bahru, Johor, Malaysia</t>
   </si>
   <si>
-    <t> +60 17 228 5068</t>
+    <t>+60 17 228 5068</t>
   </si>
   <si>
     <t>Sabah Indoor Climbing Centre</t>
@@ -348,7 +373,10 @@
     <t>Opening Hours: Mon Closed; Tue-Fri 4pm-9pm; Sat-Sun 12pm-9pm</t>
   </si>
   <si>
-    <t> +60 19 883 7341</t>
+    <t> Mon Closed; Tue-Fri 4pm-9pm; Sat-Sun 12pm-9pm</t>
+  </si>
+  <si>
+    <t>+60 19 883 7341</t>
   </si>
   <si>
     <t>https://www.facebook.com/climbsabah/</t>
@@ -357,8 +385,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -402,19 +430,112 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -722,23 +843,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C656A2AA-90BC-4C66-B420-4355AAFE936C}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{caf9cd1e-9b6d-4501-9373-df81bf09df01}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="111" customWidth="1"/>
     <col min="3" max="3" width="103" customWidth="1"/>
-    <col min="4" max="4" width="47.5546875" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
+    <col min="4" max="4" width="90.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="17.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="63.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,418 +874,476 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.75">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
       <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.75">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A21" s="2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12.75">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="F24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A25" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="12.75">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>